<commit_message>
AddRecords Class added and main.py file modified.
</commit_message>
<xml_diff>
--- a/template/template.xlsx
+++ b/template/template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Participant</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>MA</t>
   </si>
   <si>
     <t>Normal</t>
@@ -1222,7 +1225,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="100" workbookViewId="0">
       <selection activeCell="AB11" activeCellId="0" sqref="AB11"/>
     </sheetView>
   </sheetViews>
@@ -1278,7 +1281,7 @@
       <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="Q1" s="6" t="s">
@@ -1293,7 +1296,9 @@
       <c r="T1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="3"/>
+      <c r="U1" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -1310,59 +1315,61 @@
         <v>44782</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="6">
-        <f t="shared" ref="P2:P14" si="0">COUNTIF(F2:O2,0)</f>
+        <v>21</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="6">
+        <f>COUNTIF(F2:O2,0)</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="6">
-        <f t="shared" ref="Q2:Q14" si="1">COUNTIF(F2:O2,1)</f>
+      <c r="R2" s="6">
+        <f>COUNTIF(F2:O2,1)</f>
         <v>0</v>
       </c>
-      <c r="R2" s="6">
-        <f t="shared" ref="R2:R14" si="2">COUNTIF(F2:O2,2)</f>
+      <c r="S2" s="6">
+        <f>COUNTIF(F2:O2,2)</f>
         <v>0</v>
       </c>
-      <c r="S2" s="6">
-        <f t="shared" ref="S2:S14" si="3">COUNTIF(F2:O2,3)</f>
+      <c r="T2" s="6">
+        <f>COUNTIF(F2:O2,3)</f>
         <v>0</v>
       </c>
-      <c r="T2" s="6">
-        <f t="shared" ref="T2:T14" si="4">COUNTIF(F2:O2,4)</f>
+      <c r="U2" s="6">
+        <f>COUNTIF(F2:O2,4)</f>
         <v>0</v>
       </c>
-      <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -1373,59 +1380,61 @@
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="E3" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="6">
+        <f>COUNTIF(F3:O3,0)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="6">
-        <f t="shared" si="1"/>
+      <c r="R3" s="6">
+        <f>COUNTIF(F3:O3,1)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="6">
-        <f t="shared" si="2"/>
+      <c r="S3" s="6">
+        <f>COUNTIF(F3:O3,2)</f>
         <v>0</v>
       </c>
-      <c r="S3" s="6">
-        <f t="shared" si="3"/>
+      <c r="T3" s="6">
+        <f>COUNTIF(F3:O3,3)</f>
         <v>0</v>
       </c>
-      <c r="T3" s="6">
-        <f t="shared" si="4"/>
+      <c r="U3" s="6">
+        <f>COUNTIF(F3:O3,4)</f>
         <v>0</v>
       </c>
-      <c r="U3" s="3"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -1434,64 +1443,66 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="3"/>
       <c r="E4" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="6">
+        <f>COUNTIF(F4:O4,0)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="6">
-        <f t="shared" si="1"/>
+      <c r="R4" s="6">
+        <f>COUNTIF(F4:O4,1)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="6">
-        <f t="shared" si="2"/>
+      <c r="S4" s="6">
+        <f>COUNTIF(F4:O4,2)</f>
         <v>0</v>
       </c>
-      <c r="S4" s="6">
-        <f t="shared" si="3"/>
+      <c r="T4" s="6">
+        <f>COUNTIF(F4:O4,3)</f>
         <v>0</v>
       </c>
-      <c r="T4" s="6">
-        <f t="shared" si="4"/>
+      <c r="U4" s="6">
+        <f>COUNTIF(F4:O4,4)</f>
         <v>0</v>
       </c>
-      <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
@@ -1499,68 +1510,70 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="6">
+        <f>COUNTIF(F5:O5,0)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="6">
-        <f t="shared" si="1"/>
+      <c r="R5" s="6">
+        <f>COUNTIF(F5:O5,1)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="6">
-        <f t="shared" si="2"/>
+      <c r="S5" s="6">
+        <f>COUNTIF(F5:O5,2)</f>
         <v>0</v>
       </c>
-      <c r="S5" s="6">
-        <f t="shared" si="3"/>
+      <c r="T5" s="6">
+        <f>COUNTIF(F5:O5,3)</f>
         <v>0</v>
       </c>
-      <c r="T5" s="6">
-        <f t="shared" si="4"/>
+      <c r="U5" s="6">
+        <f>COUNTIF(F5:O5,4)</f>
         <v>0</v>
       </c>
-      <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
@@ -1568,71 +1581,73 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="20" t="e">
-        <f>((MAX(P2:T2)/SUM(P2:T2))+(MAX(P3:T3)/SUM(P3:T3)))/2</f>
+        <f>((MAX(Q2:U2)/SUM(Q2:U2))+(MAX(Q3:U3)/SUM(Q3:U3)))/2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="B6" s="21" t="e">
-        <f>((MAX(P4:T4)/SUM(P4:T4))+(MAX(P5:T5)/SUM(P5:T5)))/2</f>
+        <f>((MAX(Q4:U4)/SUM(Q4:U4))+(MAX(Q5:U5)/SUM(Q5:U5)))/2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C6" s="21" t="e">
-        <f>((MAX(P6:T6)/SUM(P6:T6))+(MAX(P7:T7)/SUM(P7:T7)))/2</f>
+        <f>((MAX(Q6:U6)/SUM(Q6:U6))+(MAX(Q7:U7)/SUM(Q7:U7)))/2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="6">
+        <f>COUNTIF(F6:O6,0)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="6">
-        <f t="shared" si="1"/>
+      <c r="R6" s="6">
+        <f>COUNTIF(F6:O6,1)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="6">
-        <f t="shared" si="2"/>
+      <c r="S6" s="6">
+        <f>COUNTIF(F6:O6,2)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="6">
-        <f t="shared" si="3"/>
+      <c r="T6" s="6">
+        <f>COUNTIF(F6:O6,3)</f>
         <v>0</v>
       </c>
-      <c r="T6" s="6">
-        <f t="shared" si="4"/>
+      <c r="U6" s="6">
+        <f>COUNTIF(F6:O6,4)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
@@ -1640,68 +1655,70 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="6">
+        <f>COUNTIF(F7:O7,0)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="6">
-        <f t="shared" si="1"/>
+      <c r="R7" s="6">
+        <f>COUNTIF(F7:O7,1)</f>
         <v>0</v>
       </c>
-      <c r="R7" s="6">
-        <f t="shared" si="2"/>
+      <c r="S7" s="6">
+        <f>COUNTIF(F7:O7,2)</f>
         <v>0</v>
       </c>
-      <c r="S7" s="6">
-        <f t="shared" si="3"/>
+      <c r="T7" s="6">
+        <f>COUNTIF(F7:O7,3)</f>
         <v>0</v>
       </c>
-      <c r="T7" s="6">
-        <f t="shared" si="4"/>
+      <c r="U7" s="6">
+        <f>COUNTIF(F7:O7,4)</f>
         <v>0</v>
       </c>
-      <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
@@ -1709,71 +1726,73 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="20" t="e">
-        <f>((MAX(P8:T8)/SUM(P8:T8))+(MAX(P9:T9)/SUM(P9:T9)))/2</f>
+        <f>((MAX(Q8:U8)/SUM(Q8:U8))+(MAX(Q9:U9)/SUM(Q9:U9)))/2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="B8" s="23" t="e">
-        <f>((MAX(P10:T10)/SUM(P10:T10))+(MAX(P11:T11)/SUM(P11:T11)))/2</f>
+        <f>((MAX(Q10:U10)/SUM(Q10:U10))+(MAX(Q11:U11)/SUM(Q11:U11)))/2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C8" s="23" t="e">
-        <f>((MAX(P12:T12)/SUM(P12:T12))+(MAX(P13:T13)/SUM(P13:T13)))/2</f>
+        <f>((MAX(Q12:U12)/SUM(Q12:U12))+(MAX(Q13:U13)/SUM(Q13:U13)))/2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" s="6">
+        <f>COUNTIF(F8:O8,0)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="6">
-        <f t="shared" si="1"/>
+      <c r="R8" s="6">
+        <f>COUNTIF(F8:O8,1)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="6">
-        <f t="shared" si="2"/>
+      <c r="S8" s="6">
+        <f>COUNTIF(F8:O8,2)</f>
         <v>0</v>
       </c>
-      <c r="S8" s="6">
-        <f t="shared" si="3"/>
+      <c r="T8" s="6">
+        <f>COUNTIF(F8:O8,3)</f>
         <v>0</v>
       </c>
-      <c r="T8" s="6">
-        <f t="shared" si="4"/>
+      <c r="U8" s="6">
+        <f>COUNTIF(F8:O8,4)</f>
         <v>0</v>
       </c>
-      <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
@@ -1781,68 +1800,70 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="6">
+        <f>COUNTIF(F9:O9,0)</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="6">
-        <f t="shared" si="1"/>
+      <c r="R9" s="6">
+        <f>COUNTIF(F9:O9,1)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="6">
-        <f t="shared" si="2"/>
+      <c r="S9" s="6">
+        <f>COUNTIF(F9:O9,2)</f>
         <v>0</v>
       </c>
-      <c r="S9" s="6">
-        <f t="shared" si="3"/>
+      <c r="T9" s="6">
+        <f>COUNTIF(F9:O9,3)</f>
         <v>0</v>
       </c>
-      <c r="T9" s="6">
-        <f t="shared" si="4"/>
+      <c r="U9" s="6">
+        <f>COUNTIF(F9:O9,4)</f>
         <v>0</v>
       </c>
-      <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -1850,71 +1871,73 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="26" t="e">
-        <f>((MAX(P14:T14)/SUM(P14:T14)))</f>
+        <f>((MAX(Q14:U14)/SUM(Q14:U14)))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="B10" s="25" t="str">
-        <f>_xlfn.IFS(P2=MAX(MAX(P2:T2),MAX(P3:T3)),"Normal",Q2=MAX(MAX(P2:T2),MAX(P3:T3)),"Slight",R2=MAX(MAX(P2:T2),MAX(P3:T3)),"Mild",S2=MAX(MAX(P2:T2),MAX(P3:T3)),"Moderate",T2=MAX(MAX(P2:T2),MAX(P3:T3)),"Severe",P3=MAX(MAX(P2:T2),MAX(P3:T3)),"Normal",Q3=MAX(MAX(P2:T2),MAX(P3:T3)),"Slight",R3=MAX(MAX(P2:T2),MAX(P3:T3)),"Mild",S3=MAX(MAX(P2:T2),MAX(P3:T3)),"Moderate",T3=MAX(MAX(P2:T2),MAX(P3:T3)),"Severe")</f>
+        <f>_xlfn.IFS(Q2=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Normal",R2=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Slight",S2=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Mild",T2=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Moderate",U2=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Severe",Q3=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Normal",R3=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Slight",S3=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Mild",T3=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Moderate",U3=MAX(MAX(Q2:U2),MAX(Q3:U3)),"Severe")</f>
         <v>Normal</v>
       </c>
       <c r="C10" s="27" t="str">
-        <f>_xlfn.IFS(P6=MAX(MAX(P6:T6),MAX(P7:T7)),"Normal",Q6=MAX(MAX(P6:T6),MAX(P7:T7)),"Slight",R6=MAX(MAX(P6:T6),MAX(P7:T7)),"Mild",S6=MAX(MAX(P6:T6),MAX(P7:T7)),"Moderate",T6=MAX(MAX(P6:T6),MAX(P7:T7)),"Severe",P7=MAX(MAX(P6:T6),MAX(P7:T7)),"Normal",Q7=MAX(MAX(P6:T6),MAX(P7:T7)),"Slight",R7=MAX(MAX(P6:T6),MAX(P7:T7)),"Mild",S7=MAX(MAX(P6:T6),MAX(P7:T7)),"Moderate",T7=MAX(MAX(P6:T6),MAX(P7:T7)),"Severe")</f>
+        <f>_xlfn.IFS(Q6=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Normal",R6=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Slight",S6=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Mild",T6=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Moderate",U6=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Severe",Q7=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Normal",R7=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Slight",S7=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Mild",T7=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Moderate",U7=MAX(MAX(Q6:U6),MAX(Q7:U7)),"Severe")</f>
         <v>Normal</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10" s="6">
+        <f>COUNTIF(F10:O10,0)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="6">
-        <f t="shared" si="1"/>
+      <c r="R10" s="6">
+        <f>COUNTIF(F10:O10,1)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="6">
-        <f t="shared" si="2"/>
+      <c r="S10" s="6">
+        <f>COUNTIF(F10:O10,2)</f>
         <v>0</v>
       </c>
-      <c r="S10" s="6">
-        <f t="shared" si="3"/>
+      <c r="T10" s="6">
+        <f>COUNTIF(F10:O10,3)</f>
         <v>0</v>
       </c>
-      <c r="T10" s="6">
-        <f t="shared" si="4"/>
+      <c r="U10" s="6">
+        <f>COUNTIF(F10:O10,4)</f>
         <v>0</v>
       </c>
-      <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -1922,68 +1945,70 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P11" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" s="6">
+        <f>COUNTIF(F11:O11,0)</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="6">
-        <f t="shared" si="1"/>
+      <c r="R11" s="6">
+        <f>COUNTIF(F11:O11,1)</f>
         <v>0</v>
       </c>
-      <c r="R11" s="6">
-        <f t="shared" si="2"/>
+      <c r="S11" s="6">
+        <f>COUNTIF(F11:O11,2)</f>
         <v>0</v>
       </c>
-      <c r="S11" s="6">
-        <f t="shared" si="3"/>
+      <c r="T11" s="6">
+        <f>COUNTIF(F11:O11,3)</f>
         <v>0</v>
       </c>
-      <c r="T11" s="6">
-        <f t="shared" si="4"/>
+      <c r="U11" s="6">
+        <f>COUNTIF(F11:O11,4)</f>
         <v>0</v>
       </c>
-      <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -1991,71 +2016,73 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="28" t="str">
-        <f>_xlfn.IFS(P9=MAX(P9:T9),"Normal",Q9=MAX(P9:T9),"Slight",R9=MAX(P9:T9),"Mild",S9=MAX(P9:T9),"Moderate",T9=MAX(P9:T9),"Severe")</f>
+        <f>_xlfn.IFS(Q9=MAX(Q9:U9),"Normal",R9=MAX(Q9:U9),"Slight",S9=MAX(Q9:U9),"Mild",T9=MAX(Q9:U9),"Moderate",U9=MAX(Q9:U9),"Severe")</f>
         <v>Normal</v>
       </c>
       <c r="B12" s="27" t="str">
-        <f>_xlfn.IFS(P8=MAX(MAX(P8:T8),MAX(P9:T9)),"Normal",Q8=MAX(MAX(P8:T8),MAX(P9:T9)),"Slight",R8=MAX(MAX(P8:T8),MAX(P9:T9)),"Mild",S8=MAX(MAX(P8:T8),MAX(P9:T9)),"Moderate",T8=MAX(MAX(P8:T8),MAX(P9:T9)),"Severe",P9=MAX(MAX(P8:T8),MAX(P9:T9)),"Normal",Q9=MAX(MAX(P8:T8),MAX(P9:T9)),"Slight",R9=MAX(MAX(P8:T8),MAX(P9:T9)),"Mild",S9=MAX(MAX(P8:T8),MAX(P9:T9)),"Moderate",T9=MAX(MAX(P8:T8),MAX(P9:T9)),"Severe")</f>
+        <f>_xlfn.IFS(Q8=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Normal",R8=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Slight",S8=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Mild",T8=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Moderate",U8=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Severe",Q9=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Normal",R9=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Slight",S9=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Mild",T9=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Moderate",U9=MAX(MAX(Q8:U8),MAX(Q9:U9)),"Severe")</f>
         <v>Normal</v>
       </c>
       <c r="C12" s="27" t="str">
-        <f>_xlfn.IFS(P10=MAX(MAX(P10:T10),MAX(P11:T11)),"Normal",Q10=MAX(MAX(P10:T10),MAX(P11:T11)),"Slight",R10=MAX(MAX(P10:T10),MAX(P11:T11)),"Mild",S10=MAX(MAX(P10:T10),MAX(P11:T11)),"Moderate",T10=MAX(MAX(P10:T10),MAX(P11:T11)),"Severe",P11=MAX(MAX(P10:T10),MAX(P11:T11)),"Normal",Q11=MAX(MAX(P10:T10),MAX(P11:T11)),"Slight",R11=MAX(MAX(P10:T10),MAX(P11:T11)),"Mild",S11=MAX(MAX(P10:T10),MAX(P11:T11)),"Moderate",T11=MAX(MAX(P10:T10),MAX(P11:T11)),"Severe")</f>
+        <f>_xlfn.IFS(Q10=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Normal",R10=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Slight",S10=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Mild",T10=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Moderate",U10=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Severe",Q11=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Normal",R11=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Slight",S11=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Mild",T11=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Moderate",U11=MAX(MAX(Q10:U10),MAX(Q11:U11)),"Severe")</f>
         <v>Normal</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="6">
+        <f>COUNTIF(F12:O12,0)</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="6">
-        <f t="shared" si="1"/>
+      <c r="R12" s="6">
+        <f>COUNTIF(F12:O12,1)</f>
         <v>0</v>
       </c>
-      <c r="R12" s="6">
-        <f t="shared" si="2"/>
+      <c r="S12" s="6">
+        <f>COUNTIF(F12:O12,2)</f>
         <v>0</v>
       </c>
-      <c r="S12" s="6">
-        <f t="shared" si="3"/>
+      <c r="T12" s="6">
+        <f>COUNTIF(F12:O12,3)</f>
         <v>0</v>
       </c>
-      <c r="T12" s="6">
-        <f t="shared" si="4"/>
+      <c r="U12" s="6">
+        <f>COUNTIF(F12:O12,4)</f>
         <v>0</v>
       </c>
-      <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -2063,66 +2090,68 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" s="30"/>
       <c r="E13" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" s="6">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" s="6">
+        <f>COUNTIF(F13:O13,0)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="6">
-        <f t="shared" si="1"/>
+      <c r="R13" s="6">
+        <f>COUNTIF(F13:O13,1)</f>
         <v>0</v>
       </c>
-      <c r="R13" s="6">
-        <f t="shared" si="2"/>
+      <c r="S13" s="6">
+        <f>COUNTIF(F13:O13,2)</f>
         <v>0</v>
       </c>
-      <c r="S13" s="6">
-        <f t="shared" si="3"/>
+      <c r="T13" s="6">
+        <f>COUNTIF(F13:O13,3)</f>
         <v>0</v>
       </c>
-      <c r="T13" s="6">
-        <f t="shared" si="4"/>
+      <c r="U13" s="6">
+        <f>COUNTIF(F13:O13,4)</f>
         <v>0</v>
       </c>
-      <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -2130,68 +2159,70 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="31" t="str">
-        <f>_xlfn.IFS(P12=MAX(MAX(P12:T12),MAX(P13:T13)),"Normal",Q12=MAX(MAX(P12:T12),MAX(P13:T13)),"Slight",R12=MAX(MAX(P12:T12),MAX(P13:T13)),"Mild",S12=MAX(MAX(P12:T12),MAX(P13:T13)),"Moderate",T12=MAX(MAX(P12:T12),MAX(P13:T13)),"Severe",P13=MAX(MAX(P12:T12),MAX(P13:T13)),"Normal",Q13=MAX(MAX(P12:T12),MAX(P13:T13)),"Slight",R13=MAX(MAX(P12:T12),MAX(P13:T13)),"Mild",S13=MAX(MAX(P12:T12),MAX(P13:T13)),"Moderate",T13=MAX(MAX(P12:T12),MAX(P13:T13)),"Severe")</f>
+        <f>_xlfn.IFS(Q12=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Normal",R12=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Slight",S12=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Mild",T12=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Moderate",U12=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Severe",Q13=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Normal",R13=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Slight",S13=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Mild",T13=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Moderate",U13=MAX(MAX(Q12:U12),MAX(Q13:U13)),"Severe")</f>
         <v>Normal</v>
       </c>
       <c r="B14" s="32" t="str">
-        <f>_xlfn.IFS(P14=MAX(P14:T14),"Normal",Q14=MAX(P14:T14),"Slight",R14=MAX(P14:T14),"Mild",S14=MAX(P14:T14),"Moderate",T14=MAX(P14:T14),"Severe")</f>
+        <f>_xlfn.IFS(Q14=MAX(Q14:U14),"Normal",R14=MAX(Q14:U14),"Slight",S14=MAX(Q14:U14),"Mild",T14=MAX(Q14:U14),"Moderate",U14=MAX(Q14:U14),"Severe")</f>
         <v>Normal</v>
       </c>
       <c r="C14" s="33"/>
       <c r="E14" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="34">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="34">
+        <f>COUNTIF(F14:O14,0)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="34">
-        <f t="shared" si="1"/>
+      <c r="R14" s="34">
+        <f>COUNTIF(F14:O14,1)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="34">
-        <f t="shared" si="2"/>
+      <c r="S14" s="34">
+        <f>COUNTIF(F14:O14,2)</f>
         <v>0</v>
       </c>
-      <c r="S14" s="34">
-        <f t="shared" si="3"/>
+      <c r="T14" s="34">
+        <f>COUNTIF(F14:O14,3)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="34">
-        <f t="shared" si="4"/>
+      <c r="U14" s="34">
+        <f>COUNTIF(F14:O14,4)</f>
         <v>0</v>
       </c>
-      <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>

</xml_diff>